<commit_message>
Atualização do select cimento
</commit_message>
<xml_diff>
--- a/materiais_calculados.xlsx
+++ b/materiais_calculados.xlsx
@@ -440,7 +440,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.4</v>
+        <v>4.8</v>
       </c>
     </row>
     <row r="3">
@@ -450,7 +450,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.32</v>
+        <v>18.24</v>
       </c>
     </row>
     <row r="4">
@@ -460,7 +460,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>6</v>
+        <v>72</v>
       </c>
     </row>
     <row r="5">
@@ -470,7 +470,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>8</v>
+        <v>456</v>
       </c>
     </row>
     <row r="6">
@@ -480,7 +480,7 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>192</v>
+        <v>10944</v>
       </c>
     </row>
     <row r="7">
@@ -490,7 +490,7 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>20</v>
+        <v>8</v>
       </c>
     </row>
     <row r="8">
@@ -500,7 +500,7 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>20</v>
+        <v>16</v>
       </c>
     </row>
     <row r="9">
@@ -510,7 +510,7 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>24</v>
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Atualização da formatação da planilha
</commit_message>
<xml_diff>
--- a/materiais_calculados.xlsx
+++ b/materiais_calculados.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B9"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -432,86 +432,144 @@
           <t>Quantidade</t>
         </is>
       </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>Unidade</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>Descrição</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>tinta</t>
+          <t>Tinta</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>4.8</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>litros</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>cimento</t>
+          <t>Cimento</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>18.24</v>
-      </c>
+        <v>0.8</v>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>kg</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>azulejos</t>
+          <t>Azulejos</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>72</v>
-      </c>
+        <v>30</v>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>unidades</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>areia</t>
+          <t>Areia</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>456</v>
-      </c>
+        <v>20</v>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>m³</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>tijolos</t>
+          <t>Tijolos</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>10944</v>
-      </c>
+        <v>480</v>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>unidades</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>cimento</t>
+          <t>Cimento</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>8</v>
-      </c>
+        <v>10</v>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>kg</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>areia</t>
+          <t>Areia</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>16</v>
-      </c>
+        <v>20</v>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>kg</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>pedra</t>
+          <t>Pedra</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>8</v>
-      </c>
+        <v>25</v>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>kg</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
correção de alguns bugs de biblioteca
</commit_message>
<xml_diff>
--- a/materiais_calculados.xlsx
+++ b/materiais_calculados.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D10"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -450,7 +450,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.3</v>
+        <v>1.5</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
@@ -482,7 +482,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>4.5</v>
+        <v>22.5</v>
       </c>
       <c r="C4" t="inlineStr">
         <is>
@@ -530,7 +530,7 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="C7" t="inlineStr">
         <is>
@@ -546,7 +546,7 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>108</v>
+        <v>2</v>
       </c>
       <c r="C8" t="inlineStr">
         <is>
@@ -570,22 +570,6 @@
         </is>
       </c>
       <c r="D9" t="inlineStr"/>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>Área de Aço</t>
-        </is>
-      </c>
-      <c r="B10" t="n">
-        <v>0.8812260536398466</v>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>cm²</t>
-        </is>
-      </c>
-      <c r="D10" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>